<commit_message>
feat: make API prediction load from actual trained model
</commit_message>
<xml_diff>
--- a/data/stats_table.xlsx
+++ b/data/stats_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,95 +515,114 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Lingkar Perut (cm)</t>
+          <t>BMI (Kg/m2)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>40</v>
+        <v>9.036860879904875</v>
       </c>
       <c r="C5" t="n">
-        <v>160</v>
+        <v>178.8139429606157</v>
       </c>
       <c r="D5" t="n">
-        <v>95.6318407960199</v>
+        <v>29.40742939196596</v>
       </c>
       <c r="E5" t="n">
-        <v>18.19823731823498</v>
+        <v>10.18163704002391</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Lingkar Leher (cm)</t>
+          <t>Lingkar Perut (cm)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C6" t="n">
-        <v>48</v>
+        <v>160</v>
       </c>
       <c r="D6" t="n">
-        <v>36.51741293532339</v>
+        <v>95.6318407960199</v>
       </c>
       <c r="E6" t="n">
-        <v>4.445395530217939</v>
+        <v>18.19823731823498</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Terbangun (berapa kali): buang air kecil</t>
+          <t>Lingkar Leher (cm)</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6865671641791045</v>
+        <v>36.51741293532339</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8029053581717869</v>
+        <v>4.445395530217939</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Terbangun (berapa kali): tersedak</t>
+          <t>Terbangun (berapa kali): buang air kecil</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>1.748756218905473</v>
+        <v>0.6865671641791045</v>
       </c>
       <c r="E8" t="n">
-        <v>1.793326766944895</v>
+        <v>0.8029053581717869</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>Terbangun (berapa kali): tersedak</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.748756218905473</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.793326766944895</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
           <t>Durasi tidur (jam)</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B10" t="n">
         <v>5</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>9</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>6.174129353233831</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>0.6770387061755995</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: calculate validation step
</commit_message>
<xml_diff>
--- a/data/stats_table.xlsx
+++ b/data/stats_table.xlsx
@@ -468,10 +468,10 @@
         <v>84</v>
       </c>
       <c r="D2" t="n">
-        <v>44.73134328358209</v>
+        <v>44.76674937965261</v>
       </c>
       <c r="E2" t="n">
-        <v>17.67107228487632</v>
+        <v>17.66338614348757</v>
       </c>
     </row>
     <row r="3">
@@ -487,10 +487,10 @@
         <v>185</v>
       </c>
       <c r="D3" t="n">
-        <v>164.5074626865672</v>
+        <v>164.5359801488834</v>
       </c>
       <c r="E3" t="n">
-        <v>12.52234686878205</v>
+        <v>12.51985768836525</v>
       </c>
     </row>
     <row r="4">
@@ -506,10 +506,10 @@
         <v>160</v>
       </c>
       <c r="D4" t="n">
-        <v>80.02014925373135</v>
+        <v>80.09454094292805</v>
       </c>
       <c r="E4" t="n">
-        <v>22.71208093562863</v>
+        <v>22.73292087518887</v>
       </c>
     </row>
     <row r="5">
@@ -525,10 +525,10 @@
         <v>178.8139429606157</v>
       </c>
       <c r="D5" t="n">
-        <v>29.40742939196596</v>
+        <v>29.42257563078581</v>
       </c>
       <c r="E5" t="n">
-        <v>10.18163704002391</v>
+        <v>10.17351018593594</v>
       </c>
     </row>
     <row r="6">
@@ -544,10 +544,10 @@
         <v>160</v>
       </c>
       <c r="D6" t="n">
-        <v>95.6318407960199</v>
+        <v>95.71712158808933</v>
       </c>
       <c r="E6" t="n">
-        <v>18.19823731823498</v>
+        <v>18.25603913307767</v>
       </c>
     </row>
     <row r="7">
@@ -563,10 +563,10 @@
         <v>48</v>
       </c>
       <c r="D7" t="n">
-        <v>36.51741293532339</v>
+        <v>36.52357320099256</v>
       </c>
       <c r="E7" t="n">
-        <v>4.445395530217939</v>
+        <v>4.441584937014361</v>
       </c>
     </row>
     <row r="8">
@@ -582,10 +582,10 @@
         <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6865671641791045</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8029053581717869</v>
+        <v>0.810144256311929</v>
       </c>
     </row>
     <row r="9">
@@ -601,10 +601,10 @@
         <v>6</v>
       </c>
       <c r="D9" t="n">
-        <v>1.748756218905473</v>
+        <v>1.75682382133995</v>
       </c>
       <c r="E9" t="n">
-        <v>1.793326766944895</v>
+        <v>1.798402230679146</v>
       </c>
     </row>
     <row r="10">
@@ -620,10 +620,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>6.174129353233831</v>
+        <v>6.173697270471464</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6770387061755995</v>
+        <v>0.6762517250913661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>